<commit_message>
Feat: Großer Feierabend-Push - Wetter-Icons, 5-Tage-Vorhersage und Excel-Fix fertiggestellt
</commit_message>
<xml_diff>
--- a/TestProject6/Wetter-Berichte/wetter_report.xlsx
+++ b/TestProject6/Wetter-Berichte/wetter_report.xlsx
@@ -11,6 +11,10 @@
     <sheet name="Dresden" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Berlin" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Hamburg" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="London" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Dubai" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Shenzhen" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Damaskus" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,8 +459,10 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
     <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,11 +486,21 @@
           <t>Beschreibung</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-16 09:34:55</t>
+          <t>2025-12-16 11:37:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -493,12 +509,330 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.4</v>
+        <v>1.96</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>clear sky</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="F2" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:03:35</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="F3" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:17:50</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F4" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:18:04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F5" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:18:16</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F6" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:19:24</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F7" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:21:30</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F8" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:26:54</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F9" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:44:15</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="F10" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:33:16</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="F11" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:34:44</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="F12" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:36:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F13" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-16 15:37:54</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Dresden</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F14" t="n">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,8 +856,10 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
     <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -547,11 +883,21 @@
           <t>Beschreibung</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-16 09:35:03</t>
+          <t>2025-12-16 11:37:56</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -560,12 +906,44 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2.67</v>
+        <v>4.76</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>clear sky</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="F2" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:45:46</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Berlin</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="F3" t="n">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,8 +967,10 @@
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
     <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -614,11 +994,21 @@
           <t>Beschreibung</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-16 09:35:10</t>
+          <t>2025-12-16 11:38:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -627,12 +1017,462 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3.62</v>
+        <v>6.55</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>clear sky</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="F2" t="n">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeitstempel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Stadt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Temperatur</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Beschreibung</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:38:05</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>11.68</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>overcast clouds</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="F2" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:45:21</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>11.54</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>overcast clouds</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="F3" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:48:52</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>11.48</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>overcast clouds</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="F4" t="n">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeitstempel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Stadt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Temperatur</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Beschreibung</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:38:11</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>25.96</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:04:09</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>25.96</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:44:46</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>25.96</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="F4" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeitstempel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Stadt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Temperatur</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Beschreibung</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-12-16 11:38:44</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Shenzhen</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>21.28</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>broken clouds</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="F2" t="n">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Zeitstempel</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Stadt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Temperatur</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Beschreibung</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Windgeschwindkeit</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luftfeuchtigkeit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-12-16 13:53:44</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Damaskus</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>overcast clouds</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="F2" t="n">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>